<commit_message>
feat: 自动添加每日生成文件 AIPEEarningYield.xlsx (Colab)
</commit_message>
<xml_diff>
--- a/data/AIPEEarningYield.xlsx
+++ b/data/AIPEEarningYield.xlsx
@@ -684,7 +684,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>33.99999999999982</v>
+        <v>33.99999999999983</v>
       </c>
       <c r="E7" t="n">
         <v>2281.879194630872</v>
@@ -693,7 +693,7 @@
         <v>29.8</v>
       </c>
       <c r="G7" t="n">
-        <v>67999.99999999999</v>
+        <v>68000</v>
       </c>
       <c r="H7" t="n">
         <v>200000</v>
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>49.99999999999976</v>
+        <v>49.99999999999975</v>
       </c>
       <c r="E5" t="n">
         <v>1745.810055865922</v>
@@ -1269,7 +1269,7 @@
         <v>75.25</v>
       </c>
       <c r="G7" t="n">
-        <v>30000.00000000001</v>
+        <v>30000</v>
       </c>
       <c r="H7" t="n">
         <v>200000</v>
@@ -1306,7 +1306,7 @@
         <v>29.8</v>
       </c>
       <c r="G8" t="n">
-        <v>40000.00000000001</v>
+        <v>40000</v>
       </c>
       <c r="H8" t="n">
         <v>200000</v>

</xml_diff>